<commit_message>
ORG Cache First round of Test script completed 150 records already sent to manual tester for validation
</commit_message>
<xml_diff>
--- a/src/test/testdata/ORG_Website_Cache_File.xlsx
+++ b/src/test/testdata/ORG_Website_Cache_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R3_Project\R3_Report_Automation\src\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874B21A7-A18D-4A43-AD3C-A20003A4B3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811BBA5D-995B-4151-AB3E-9E9BE9076550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5893,9 +5893,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5933,7 +5933,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6039,7 +6039,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6181,7 +6181,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6192,12 +6192,16 @@
   <dimension ref="A1:E685"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>